<commit_message>
finally,we do some work with java
</commit_message>
<xml_diff>
--- a/doc/database_structure.xlsx
+++ b/doc/database_structure.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="113">
   <si>
     <t>content</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -454,6 +454,18 @@
   </si>
   <si>
     <t>热门</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>the_order</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reserved</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>预留字段</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -798,10 +810,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:C50"/>
+  <dimension ref="A2:C51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+      <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -897,304 +909,312 @@
     </row>
     <row r="12" spans="1:3">
       <c r="B12" t="s">
-        <v>57</v>
+        <v>110</v>
       </c>
       <c r="C12" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>67</v>
-      </c>
-      <c r="B14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" t="s">
-        <v>59</v>
+    <row r="13" spans="1:3">
+      <c r="B13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
         <v>99</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>1</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="B16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="B17" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="B18" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="B19" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>94</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="B20" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="B21" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="B22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="B24" t="s">
         <v>57</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>61</v>
-      </c>
-      <c r="B25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
         <v>98</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>7</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="B27" t="s">
-        <v>105</v>
-      </c>
-      <c r="C27" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="B28" t="s">
-        <v>4</v>
+        <v>105</v>
       </c>
       <c r="C28" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="B29" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="B30" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C30" t="s">
-        <v>94</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="B31" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>53</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="B32" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="B33" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="B34" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C34" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="B35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="B36" t="s">
         <v>57</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
-        <v>65</v>
-      </c>
-      <c r="B37" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
         <v>68</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>70</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="B39" t="s">
-        <v>72</v>
-      </c>
-      <c r="C39" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="B40" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C40" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="B41" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C41" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="B42" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="B43" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C43" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="B44" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C44" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="B45" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C45" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="B46" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="C46" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="B47" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C47" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="B48" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="C48" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="49" spans="2:3">
       <c r="B49" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C49" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="50" spans="2:3">
       <c r="B50" t="s">
+        <v>74</v>
+      </c>
+      <c r="C50" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3">
+      <c r="B51" t="s">
         <v>86</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C51" t="s">
         <v>85</v>
       </c>
     </row>

</xml_diff>